<commit_message>
MealTest finished, classes updated
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="19380" windowHeight="6435"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19380" windowHeight="6435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Meal Search Results" sheetId="1" r:id="rId1"/>
     <sheet name="Meals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:J19"/>
+  <oleSize ref="A1:I19"/>
 </workbook>
 </file>
 
@@ -429,7 +429,9 @@
   </sheetPr>
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -672,8 +674,8 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
SearchResultPage and SearchTest added
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Meals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:J19"/>
+  <oleSize ref="A1:D19"/>
 </workbook>
 </file>
 
@@ -430,7 +430,7 @@
   <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -660,8 +660,8 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -675,7 +675,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>